<commit_message>
create_user, write user script
</commit_message>
<xml_diff>
--- a/ue01_useranlegen/users.xlsx
+++ b/ue01_useranlegen/users.xlsx
@@ -501,7 +501,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Maximilian#De_Junious(2cn=</t>
+          <t>Maximilian,De_Junious#2cn=</t>
         </is>
       </c>
     </row>
@@ -528,7 +528,7 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>Ramon=Nunez_Gomez,3bn=</t>
+          <t>Ramon!Nunez_Gomez%3bn!</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>Uelkue_Oemer-Uellaegoess_1an#</t>
+          <t>Uelkue_Oemer=Uellaegoess=1an#</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>Isis(Lanpher(4cn(</t>
+          <t>Isis#Lanpher)4cn(</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>Maximilian,Galvin#2an%</t>
+          <t>Maximilian%Galvin=2an=</t>
         </is>
       </c>
     </row>
@@ -636,7 +636,7 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>Jannette_Laspina#4cn.</t>
+          <t>Jannette,Laspina-4cn(</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>Marg_Dodich^3cn#</t>
+          <t>Marg)Dodich-3cn(</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>Carisa.Bannowsky(2an=</t>
+          <t>Carisa!Bannowsky!2an)</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>David(Waisath)4cn)</t>
+          <t>David,Waisath&amp;4cn=</t>
         </is>
       </c>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>Paulette!von_Reddig-Piette=2cn.</t>
+          <t>Paulette^von_Reddig-Piette=2cn#</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>Kirby,Latona(2an-</t>
+          <t>Kirby!Latona.2an,</t>
         </is>
       </c>
     </row>
@@ -798,7 +798,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>Reed(Homewood^2bn(</t>
+          <t>Reed)Homewood(2bn!</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>Blair-Pallafor-Zedian%5cn&amp;</t>
+          <t>Blair^Pallafor-Zedian_5cn_</t>
         </is>
       </c>
     </row>
@@ -852,7 +852,7 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>Lon_Senemounnarat-Quillian#2cn%</t>
+          <t>Lon=Senemounnarat-Quillian#2cn-</t>
         </is>
       </c>
     </row>
@@ -879,7 +879,7 @@
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Vada^Isaac.2bn,</t>
+          <t>Vada%Isaac(2bn&amp;</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>Jeanett(Plancarte&amp;4bn-</t>
+          <t>Jeanett_Plancarte-4bn,</t>
         </is>
       </c>
     </row>
@@ -929,7 +929,7 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Alex!Berteotti-Stirn-None%</t>
+          <t>Alex)Berteotti-Stirn(None&amp;</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>Robyn^Strycker.3an%</t>
+          <t>Robyn%Strycker,3an!</t>
         </is>
       </c>
     </row>
@@ -983,7 +983,7 @@
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Camille,Von_Verrill^3bn,</t>
+          <t>Camille#Von_Verrill(3bn^</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>Franz_Michael_Leopold%Deschner^4cn^</t>
+          <t>Franz_Michael_Leopold&amp;Deschner!4cn)</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Veola%Franzi=None%</t>
+          <t>Veola%Franzi%None.</t>
         </is>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>Chantelle%Cringle^3cn!</t>
+          <t>Chantelle=Cringle%3cn%</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>Britney_Kosh.5bn&amp;</t>
+          <t>Britney%Kosh!5bn=</t>
         </is>
       </c>
     </row>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>Clayton.Derouchie=4bn&amp;</t>
+          <t>Clayton^Derouchie%4bn%</t>
         </is>
       </c>
     </row>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>Beverlee^Doutt&amp;5bn)</t>
+          <t>Beverlee&amp;Doutt,5bn%</t>
         </is>
       </c>
     </row>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>Alma%Munley!1bn#</t>
+          <t>Alma)Munley&amp;1bn#</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>Thad)Dornbos.5an.</t>
+          <t>Thad(Dornbos)5an,</t>
         </is>
       </c>
     </row>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>Arvilla%Mahala&amp;2cn)</t>
+          <t>Arvilla&amp;Mahala,2cn-</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>Mirza^Ellingwood.None!</t>
+          <t>Mirza!Ellingwood,None&amp;</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>Francie^de_Cardinalli-Sciola^3an,</t>
+          <t>Francie(de_Cardinalli-Sciola,3an&amp;</t>
         </is>
       </c>
     </row>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>IRENEE=Gundry%None&amp;</t>
+          <t>IRENEE_Gundry&amp;None&amp;</t>
         </is>
       </c>
     </row>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>IRENEE&amp;Pinedo.3cn)</t>
+          <t>IRENEE!Pinedo)3cn)</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>Mirza,Pinsky(1bn,</t>
+          <t>Mirza,Pinsky#1bn#</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>Francie(Pinsky1#1bn#</t>
+          <t>Francie-Pinsky1^1bn_</t>
         </is>
       </c>
     </row>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>Goldie-Pinsky2&amp;1bn-</t>
+          <t>Goldie=Pinsky2-1bn,</t>
         </is>
       </c>
     </row>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>A-nother,Pinsky3(1bn-</t>
+          <t>A-nother#Pinsky3(1bn^</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ue01_useranlegen, a bit of refactoring, tests and write_txt
</commit_message>
<xml_diff>
--- a/ue01_useranlegen/users.xlsx
+++ b/ue01_useranlegen/users.xlsx
@@ -501,7 +501,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Maximilian,De_Junious#2cn=</t>
+          <t>Maximilian.De_Junious&amp;2cn,</t>
         </is>
       </c>
     </row>
@@ -528,7 +528,7 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>Ramon!Nunez_Gomez%3bn!</t>
+          <t>Ramon,Nunez_Gomez=3bn=</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>Uelkue_Oemer=Uellaegoess=1an#</t>
+          <t>Uelkue_Oemer,Uellaegoess^1an-</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>Isis#Lanpher)4cn(</t>
+          <t>Isis(Lanpher!4cn,</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>Maximilian%Galvin=2an=</t>
+          <t>Maximilian-Galvin-2an(</t>
         </is>
       </c>
     </row>
@@ -636,7 +636,7 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>Jannette,Laspina-4cn(</t>
+          <t>Jannette(Laspina#4cn&amp;</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>Marg)Dodich-3cn(</t>
+          <t>Marg#Dodich&amp;3cn.</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>Carisa!Bannowsky!2an)</t>
+          <t>Carisa&amp;Bannowsky^2an(</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>David,Waisath&amp;4cn=</t>
+          <t>David)Waisath^4cn-</t>
         </is>
       </c>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>Paulette^von_Reddig-Piette=2cn#</t>
+          <t>Paulette&amp;von_Reddig-Piette#2cn-</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>Kirby!Latona.2an,</t>
+          <t>Kirby!Latona(2an&amp;</t>
         </is>
       </c>
     </row>
@@ -798,7 +798,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>Reed)Homewood(2bn!</t>
+          <t>Reed,Homewood)2bn#</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>Blair^Pallafor-Zedian_5cn_</t>
+          <t>Blair-Pallafor-Zedian^5cn_</t>
         </is>
       </c>
     </row>
@@ -852,7 +852,7 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>Lon=Senemounnarat-Quillian#2cn-</t>
+          <t>Lon.Senemounnarat-Quillian!2cn_</t>
         </is>
       </c>
     </row>
@@ -879,7 +879,7 @@
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Vada%Isaac(2bn&amp;</t>
+          <t>Vada(Isaac(2bn=</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>Jeanett_Plancarte-4bn,</t>
+          <t>Jeanett,Plancarte-4bn.</t>
         </is>
       </c>
     </row>
@@ -929,7 +929,7 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Alex)Berteotti-Stirn(None&amp;</t>
+          <t>Alex^Berteotti-Stirn.None&amp;</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>Robyn%Strycker,3an!</t>
+          <t>Robyn%Strycker_3an_</t>
         </is>
       </c>
     </row>
@@ -983,7 +983,7 @@
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Camille#Von_Verrill(3bn^</t>
+          <t>Camille!Von_Verrill^3bn%</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>Franz_Michael_Leopold&amp;Deschner!4cn)</t>
+          <t>Franz_Michael_Leopold#Deschner(4cn,</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Veola%Franzi%None.</t>
+          <t>Veola%Franzi(None&amp;</t>
         </is>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>Chantelle=Cringle%3cn%</t>
+          <t>Chantelle)Cringle_3cn#</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>Britney%Kosh!5bn=</t>
+          <t>Britney_Kosh-5bn.</t>
         </is>
       </c>
     </row>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>Clayton^Derouchie%4bn%</t>
+          <t>Clayton_Derouchie)4bn.</t>
         </is>
       </c>
     </row>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>Beverlee&amp;Doutt,5bn%</t>
+          <t>Beverlee^Doutt=5bn-</t>
         </is>
       </c>
     </row>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>Alma)Munley&amp;1bn#</t>
+          <t>Alma,Munley.1bn(</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>Thad(Dornbos)5an,</t>
+          <t>Thad!Dornbos=5an!</t>
         </is>
       </c>
     </row>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>Arvilla&amp;Mahala,2cn-</t>
+          <t>Arvilla)Mahala)2cn!</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>Mirza!Ellingwood,None&amp;</t>
+          <t>Mirza_Ellingwood-None,</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>Francie(de_Cardinalli-Sciola,3an&amp;</t>
+          <t>Francie!de_Cardinalli-Sciola(3an#</t>
         </is>
       </c>
     </row>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>IRENEE_Gundry&amp;None&amp;</t>
+          <t>IRENEE%Gundry=None.</t>
         </is>
       </c>
     </row>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>IRENEE!Pinedo)3cn)</t>
+          <t>IRENEE-Pinedo%3cn=</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>Mirza,Pinsky#1bn#</t>
+          <t>Mirza!Pinsky^1bn,</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>Francie-Pinsky1^1bn_</t>
+          <t>Francie^Pinsky1_1bn&amp;</t>
         </is>
       </c>
     </row>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>Goldie=Pinsky2-1bn,</t>
+          <t>Goldie%Pinsky2-1bn^</t>
         </is>
       </c>
     </row>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>A-nother#Pinsky3(1bn^</t>
+          <t>A-nother!Pinsky3=1bn,</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ue01_useranlegen, small changes to write_txt
</commit_message>
<xml_diff>
--- a/ue01_useranlegen/users.xlsx
+++ b/ue01_useranlegen/users.xlsx
@@ -501,7 +501,7 @@
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>Maximilian.De_Junious&amp;2cn,</t>
+          <t>Maximilian_De_Junious(2cn)</t>
         </is>
       </c>
     </row>
@@ -528,7 +528,7 @@
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t>Ramon,Nunez_Gomez=3bn=</t>
+          <t>Ramon#Nunez_Gomez&amp;3bn=</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>Uelkue_Oemer,Uellaegoess^1an-</t>
+          <t>Uelkue_Oemer)Uellaegoess)1an&amp;</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t>Isis(Lanpher!4cn,</t>
+          <t>Isis_Lanpher!4cn,</t>
         </is>
       </c>
     </row>
@@ -609,7 +609,7 @@
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>Maximilian-Galvin-2an(</t>
+          <t>Maximilian-Galvin_2an!</t>
         </is>
       </c>
     </row>
@@ -636,7 +636,7 @@
       </c>
       <c r="E7" s="3" t="inlineStr">
         <is>
-          <t>Jannette(Laspina#4cn&amp;</t>
+          <t>Jannette(Laspina!4cn#</t>
         </is>
       </c>
     </row>
@@ -663,7 +663,7 @@
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
-          <t>Marg#Dodich&amp;3cn.</t>
+          <t>Marg(Dodich)3cn)</t>
         </is>
       </c>
     </row>
@@ -690,7 +690,7 @@
       </c>
       <c r="E9" s="3" t="inlineStr">
         <is>
-          <t>Carisa&amp;Bannowsky^2an(</t>
+          <t>Carisa.Bannowsky,2an.</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>David)Waisath^4cn-</t>
+          <t>David^Waisath_4cn,</t>
         </is>
       </c>
     </row>
@@ -744,7 +744,7 @@
       </c>
       <c r="E11" s="3" t="inlineStr">
         <is>
-          <t>Paulette&amp;von_Reddig-Piette#2cn-</t>
+          <t>Paulette=von_Reddig-Piette(2cn=</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>Kirby!Latona(2an&amp;</t>
+          <t>Kirby(Latona!2an%</t>
         </is>
       </c>
     </row>
@@ -798,7 +798,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t>Reed,Homewood)2bn#</t>
+          <t>Reed#Homewood,2bn(</t>
         </is>
       </c>
     </row>
@@ -825,7 +825,7 @@
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>Blair-Pallafor-Zedian^5cn_</t>
+          <t>Blair.Pallafor-Zedian-5cn_</t>
         </is>
       </c>
     </row>
@@ -852,7 +852,7 @@
       </c>
       <c r="E15" s="3" t="inlineStr">
         <is>
-          <t>Lon.Senemounnarat-Quillian!2cn_</t>
+          <t>Lon=Senemounnarat-Quillian#2cn%</t>
         </is>
       </c>
     </row>
@@ -879,7 +879,7 @@
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>Vada(Isaac(2bn=</t>
+          <t>Vada.Isaac-2bn_</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="E17" s="3" t="inlineStr">
         <is>
-          <t>Jeanett,Plancarte-4bn.</t>
+          <t>Jeanett!Plancarte-4bn,</t>
         </is>
       </c>
     </row>
@@ -929,7 +929,7 @@
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>Alex^Berteotti-Stirn.None&amp;</t>
+          <t>Alex,Berteotti-Stirn-l3hr3r%</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="E19" s="3" t="inlineStr">
         <is>
-          <t>Robyn%Strycker_3an_</t>
+          <t>Robyn!Strycker&amp;3an%</t>
         </is>
       </c>
     </row>
@@ -983,7 +983,7 @@
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>Camille!Von_Verrill^3bn%</t>
+          <t>Camille^Von_Verrill%3bn(</t>
         </is>
       </c>
     </row>
@@ -1010,7 +1010,7 @@
       </c>
       <c r="E21" s="3" t="inlineStr">
         <is>
-          <t>Franz_Michael_Leopold#Deschner(4cn,</t>
+          <t>Franz_Michael_Leopold)Deschner-4cn.</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>Veola%Franzi(None&amp;</t>
+          <t>Veola=Franzi#l3hr3r=</t>
         </is>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t>Chantelle)Cringle_3cn#</t>
+          <t>Chantelle-Cringle%3cn!</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>Britney_Kosh-5bn.</t>
+          <t>Britney#Kosh(5bn%</t>
         </is>
       </c>
     </row>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="E25" s="3" t="inlineStr">
         <is>
-          <t>Clayton_Derouchie)4bn.</t>
+          <t>Clayton^Derouchie^4bn&amp;</t>
         </is>
       </c>
     </row>
@@ -1141,7 +1141,7 @@
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>Beverlee^Doutt=5bn-</t>
+          <t>Beverlee%Doutt(5bn(</t>
         </is>
       </c>
     </row>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t>Alma,Munley.1bn(</t>
+          <t>Alma%Munley!1bn#</t>
         </is>
       </c>
     </row>
@@ -1195,7 +1195,7 @@
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>Thad!Dornbos=5an!</t>
+          <t>Thad,Dornbos-5an(</t>
         </is>
       </c>
     </row>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t>Arvilla)Mahala)2cn!</t>
+          <t>Arvilla_Mahala&amp;2cn&amp;</t>
         </is>
       </c>
     </row>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>Mirza_Ellingwood-None,</t>
+          <t>Mirza)Ellingwood(l3hr3r!</t>
         </is>
       </c>
     </row>
@@ -1272,7 +1272,7 @@
       </c>
       <c r="E31" s="3" t="inlineStr">
         <is>
-          <t>Francie!de_Cardinalli-Sciola(3an#</t>
+          <t>Francie%de_Cardinalli-Sciola.3an#</t>
         </is>
       </c>
     </row>
@@ -1295,7 +1295,7 @@
       </c>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>IRENEE%Gundry=None.</t>
+          <t>IRENEE#Gundry^l3hr3r_</t>
         </is>
       </c>
     </row>
@@ -1322,7 +1322,7 @@
       </c>
       <c r="E33" s="3" t="inlineStr">
         <is>
-          <t>IRENEE-Pinedo%3cn=</t>
+          <t>IRENEE,Pinedo(3cn-</t>
         </is>
       </c>
     </row>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>Mirza!Pinsky^1bn,</t>
+          <t>Mirza-Pinsky!1bn!</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="E35" s="3" t="inlineStr">
         <is>
-          <t>Francie^Pinsky1_1bn&amp;</t>
+          <t>Francie=Pinsky1&amp;1bn-</t>
         </is>
       </c>
     </row>
@@ -1403,7 +1403,7 @@
       </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>Goldie%Pinsky2-1bn^</t>
+          <t>Goldie=Pinsky2(1bn)</t>
         </is>
       </c>
     </row>
@@ -1430,7 +1430,7 @@
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t>A-nother!Pinsky3=1bn,</t>
+          <t>A-nother-Pinsky3^1bn^</t>
         </is>
       </c>
     </row>

</xml_diff>